<commit_message>
nuevo script y mas datos consumo y distancia al excel
</commit_message>
<xml_diff>
--- a/plazas_seccion.xlsx
+++ b/plazas_seccion.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Program Files\Aimsun\Aimsun Next 8.3\programming\Aimsun Next API\AAPIPython\Micro\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tablet\Documents\GitHub\Aparcamientos---py\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E6964A9-38EE-4B81-8A34-09A370B09ED9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67538017-AB5B-4315-B4D4-74E08F694064}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4B658B76-A982-4A03-A763-6FD68BFBB064}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{4B658B76-A982-4A03-A763-6FD68BFBB064}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -396,13 +398,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E4179AE-46D8-4A45-9FDF-47BA471CB764}">
   <dimension ref="A1:D97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -416,7 +418,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>862</v>
       </c>
@@ -431,7 +433,7 @@
         <v>9.5238095238095247E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>865</v>
       </c>
@@ -446,7 +448,7 @@
         <v>1.2698412698412698E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>869</v>
       </c>
@@ -458,7 +460,7 @@
         <v>6.3492063492063492E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>874</v>
       </c>
@@ -470,7 +472,7 @@
         <v>6.3492063492063492E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>877</v>
       </c>
@@ -479,7 +481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>879</v>
       </c>
@@ -491,7 +493,7 @@
         <v>1.5873015873015872E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>882</v>
       </c>
@@ -503,7 +505,7 @@
         <v>6.3492063492063492E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>887</v>
       </c>
@@ -515,7 +517,7 @@
         <v>6.3492063492063492E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>889</v>
       </c>
@@ -530,7 +532,7 @@
         <v>5.7142857142857141E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>892</v>
       </c>
@@ -545,7 +547,7 @@
         <v>6.9841269841269843E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>893</v>
       </c>
@@ -560,7 +562,7 @@
         <v>8.2539682539682538E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>895</v>
       </c>
@@ -575,7 +577,7 @@
         <v>4.7619047619047616E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>896</v>
       </c>
@@ -584,7 +586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>899</v>
       </c>
@@ -599,7 +601,7 @@
         <v>2.2222222222222223E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>901</v>
       </c>
@@ -614,7 +616,7 @@
         <v>1.9047619047619049E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>903</v>
       </c>
@@ -623,7 +625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>911</v>
       </c>
@@ -632,7 +634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>914</v>
       </c>
@@ -641,7 +643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>927</v>
       </c>
@@ -650,7 +652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>928</v>
       </c>
@@ -659,7 +661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>929</v>
       </c>
@@ -668,7 +670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>932</v>
       </c>
@@ -677,7 +679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>934</v>
       </c>
@@ -692,7 +694,7 @@
         <v>3.8095238095238099E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>937</v>
       </c>
@@ -701,7 +703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>939</v>
       </c>
@@ -710,7 +712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>944</v>
       </c>
@@ -719,7 +721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>946</v>
       </c>
@@ -734,7 +736,7 @@
         <v>1.9047619047619049E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>948</v>
       </c>
@@ -743,7 +745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>961</v>
       </c>
@@ -752,7 +754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>963</v>
       </c>
@@ -761,7 +763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>968</v>
       </c>
@@ -776,7 +778,7 @@
         <v>4.7619047619047616E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>971</v>
       </c>
@@ -785,7 +787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>981</v>
       </c>
@@ -794,7 +796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>983</v>
       </c>
@@ -803,7 +805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>985</v>
       </c>
@@ -812,7 +814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>988</v>
       </c>
@@ -821,7 +823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>992</v>
       </c>
@@ -836,7 +838,7 @@
         <v>6.3492063492063492E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>994</v>
       </c>
@@ -845,7 +847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>996</v>
       </c>
@@ -854,7 +856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>998</v>
       </c>
@@ -869,7 +871,7 @@
         <v>9.5238095238095247E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>1005</v>
       </c>
@@ -878,7 +880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>1008</v>
       </c>
@@ -887,7 +889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>1010</v>
       </c>
@@ -896,7 +898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>1011</v>
       </c>
@@ -905,7 +907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>1016</v>
       </c>
@@ -914,7 +916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>1018</v>
       </c>
@@ -923,7 +925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>1019</v>
       </c>
@@ -932,7 +934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>1020</v>
       </c>
@@ -941,7 +943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>1021</v>
       </c>
@@ -950,7 +952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>1024</v>
       </c>
@@ -959,7 +961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>1025</v>
       </c>
@@ -968,7 +970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>1026</v>
       </c>
@@ -977,7 +979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>1033</v>
       </c>
@@ -986,7 +988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>1037</v>
       </c>
@@ -995,7 +997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>1042</v>
       </c>
@@ -1010,7 +1012,7 @@
         <v>2.2222222222222223E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>1043</v>
       </c>
@@ -1025,7 +1027,7 @@
         <v>5.7142857142857141E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>1047</v>
       </c>
@@ -1040,7 +1042,7 @@
         <v>1.9047619047619049E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>1049</v>
       </c>
@@ -1052,7 +1054,7 @@
         <v>5.0793650793650794E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>1056</v>
       </c>
@@ -1067,13 +1069,10 @@
         <v>1.5873015873015872E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>1058</v>
       </c>
-      <c r="B61">
-        <v>0</v>
-      </c>
       <c r="C61">
         <v>16</v>
       </c>
@@ -1082,7 +1081,7 @@
         <v>5.0793650793650794E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>1059</v>
       </c>
@@ -1097,7 +1096,7 @@
         <v>6.3492063492063489E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>1063</v>
       </c>
@@ -1112,7 +1111,7 @@
         <v>3.4920634920634921E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>1066</v>
       </c>
@@ -1124,7 +1123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>1078</v>
       </c>
@@ -1139,7 +1138,7 @@
         <v>5.7142857142857141E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>1079</v>
       </c>
@@ -1148,7 +1147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>1085</v>
       </c>
@@ -1163,7 +1162,7 @@
         <v>3.8095238095238099E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>1086</v>
       </c>
@@ -1172,7 +1171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>1089</v>
       </c>
@@ -1187,7 +1186,7 @@
         <v>5.0793650793650794E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>1092</v>
       </c>
@@ -1202,7 +1201,7 @@
         <v>4.1269841269841269E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>1095</v>
       </c>
@@ -1211,7 +1210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>1101</v>
       </c>
@@ -1220,7 +1219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>1103</v>
       </c>
@@ -1229,7 +1228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>1106</v>
       </c>
@@ -1238,7 +1237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>1109</v>
       </c>
@@ -1247,7 +1246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>1126</v>
       </c>
@@ -1256,7 +1255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>1129</v>
       </c>
@@ -1271,7 +1270,7 @@
         <v>1.5873015873015872E-2</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>1131</v>
       </c>
@@ -1280,7 +1279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>1146</v>
       </c>
@@ -1289,7 +1288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>1148</v>
       </c>
@@ -1298,7 +1297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>1156</v>
       </c>
@@ -1307,7 +1306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>1158</v>
       </c>
@@ -1316,7 +1315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>1161</v>
       </c>
@@ -1325,7 +1324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>1164</v>
       </c>
@@ -1334,7 +1333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>1165</v>
       </c>
@@ -1343,7 +1342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>1169</v>
       </c>
@@ -1352,7 +1351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>1176</v>
       </c>
@@ -1361,7 +1360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>1178</v>
       </c>
@@ -1370,7 +1369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>1237</v>
       </c>
@@ -1379,7 +1378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>1246</v>
       </c>
@@ -1388,7 +1387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>1249</v>
       </c>
@@ -1397,7 +1396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>1276</v>
       </c>
@@ -1406,7 +1405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>1294</v>
       </c>
@@ -1415,7 +1414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>1297</v>
       </c>
@@ -1424,7 +1423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>1300</v>
       </c>
@@ -1433,7 +1432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>1306</v>
       </c>
@@ -1442,7 +1441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>1309</v>
       </c>

</xml_diff>